<commit_message>
Cambio cabeceras a castellano
</commit_message>
<xml_diff>
--- a/datos/entrada/19.xlsx
+++ b/datos/entrada/19.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\CALCULADORADOCENTES\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\CALCULADORADOCENTES\datos\entrada\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F6AF68A8-A78E-4B51-BF9A-886588F3C72B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03948E20-E8A2-44CC-B650-479483BF6551}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{F81BB5CD-81A5-47AE-A663-66CD959ED930}"/>
+    <workbookView xWindow="22932" yWindow="-36" windowWidth="23256" windowHeight="12576" xr2:uid="{F81BB5CD-81A5-47AE-A663-66CD959ED930}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -38,24 +38,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="358" uniqueCount="264">
   <si>
-    <t>Codi</t>
-  </si>
-  <si>
-    <t>Centre</t>
-  </si>
-  <si>
-    <t>Règ.</t>
-  </si>
-  <si>
-    <t>Adreça</t>
-  </si>
-  <si>
-    <t>Localitat</t>
-  </si>
-  <si>
-    <t>Telèfon</t>
-  </si>
-  <si>
     <t>IES PORÇONS</t>
   </si>
   <si>
@@ -828,6 +810,24 @@
   </si>
   <si>
     <t>Avda. DE LES CORTS VALENCIANES, S/N</t>
+  </si>
+  <si>
+    <t>Código</t>
+  </si>
+  <si>
+    <t>Centro</t>
+  </si>
+  <si>
+    <t>Rég.</t>
+  </si>
+  <si>
+    <t>Dirección</t>
+  </si>
+  <si>
+    <t>Localidad</t>
+  </si>
+  <si>
+    <t>Teléfono</t>
   </si>
 </sst>
 </file>
@@ -874,13 +874,13 @@
   </cellStyleXfs>
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -890,22 +890,7 @@
   </cellStyles>
   <dxfs count="8">
     <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <fill>
@@ -961,6 +946,15 @@
       </fill>
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -975,15 +969,15 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{BB7EC161-8E62-487A-8C66-04C4069F6419}" name="Table2" displayName="Table2" ref="A1:F89" totalsRowShown="0" headerRowDxfId="0" dataDxfId="1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{BB7EC161-8E62-487A-8C66-04C4069F6419}" name="Table2" displayName="Table2" ref="A1:F89" totalsRowShown="0" headerRowDxfId="0" dataDxfId="7">
   <autoFilter ref="A1:F89" xr:uid="{BB7EC161-8E62-487A-8C66-04C4069F6419}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{9075C1E5-F1A4-4476-8C24-C8092C642D49}" name="Codi" dataDxfId="7" dataCellStyle="Hyperlink"/>
-    <tableColumn id="2" xr3:uid="{2138F0DE-1B17-4413-B4B2-B29933D88C35}" name="Centre" dataDxfId="6"/>
-    <tableColumn id="3" xr3:uid="{61841238-050C-4EE7-8A5E-7D131B661B16}" name="Règ." dataDxfId="5"/>
-    <tableColumn id="4" xr3:uid="{1BF81DEE-5237-49ED-BBE8-62CE3DD7D3FB}" name="Adreça" dataDxfId="4"/>
-    <tableColumn id="5" xr3:uid="{4E9768B4-1243-47B8-8D50-906D0A0CF6DE}" name="Localitat" dataDxfId="3"/>
-    <tableColumn id="6" xr3:uid="{D10DEE69-D34B-4992-8A76-876C639456EE}" name="Telèfon" dataDxfId="2"/>
+    <tableColumn id="1" xr3:uid="{9075C1E5-F1A4-4476-8C24-C8092C642D49}" name="Código" dataDxfId="6" dataCellStyle="Hyperlink"/>
+    <tableColumn id="2" xr3:uid="{2138F0DE-1B17-4413-B4B2-B29933D88C35}" name="Centro" dataDxfId="5"/>
+    <tableColumn id="3" xr3:uid="{61841238-050C-4EE7-8A5E-7D131B661B16}" name="Rég." dataDxfId="4"/>
+    <tableColumn id="4" xr3:uid="{1BF81DEE-5237-49ED-BBE8-62CE3DD7D3FB}" name="Dirección" dataDxfId="3"/>
+    <tableColumn id="5" xr3:uid="{4E9768B4-1243-47B8-8D50-906D0A0CF6DE}" name="Localidad" dataDxfId="2"/>
+    <tableColumn id="6" xr3:uid="{D10DEE69-D34B-4992-8A76-876C639456EE}" name="Teléfono" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1309,7 +1303,7 @@
   <dimension ref="A1:F89"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C87" sqref="C87"/>
+      <selection sqref="A1:F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1324,22 +1318,22 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>0</v>
+        <v>258</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>1</v>
+        <v>259</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>2</v>
+        <v>260</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>3</v>
+        <v>261</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>4</v>
+        <v>262</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>5</v>
+        <v>263</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -1347,16 +1341,16 @@
         <v>3001881</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="F2" s="3">
         <v>965936490</v>
@@ -1367,16 +1361,16 @@
         <v>3001911</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="F3" s="3">
         <v>965936500</v>
@@ -1387,16 +1381,16 @@
         <v>3002445</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="F4" s="3">
         <v>966926770</v>
@@ -1407,16 +1401,16 @@
         <v>3003978</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="F5" s="3">
         <v>966912225</v>
@@ -1427,36 +1421,36 @@
         <v>3004223</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="F6" s="3">
         <v>966428225</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>3005094</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="F7" s="3">
         <v>966912235</v>
@@ -1467,16 +1461,16 @@
         <v>3006761</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
       <c r="F8" s="3">
         <v>966908115</v>
@@ -1487,16 +1481,16 @@
         <v>3007613</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>180</v>
+        <v>174</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
       <c r="F9" s="3">
         <v>966409960</v>
@@ -1507,16 +1501,16 @@
         <v>3008423</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>200</v>
+        <v>194</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>201</v>
+        <v>195</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>202</v>
+        <v>196</v>
       </c>
       <c r="F10" s="3">
         <v>965936505</v>
@@ -1527,16 +1521,16 @@
         <v>3008915</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
       <c r="F11" s="3">
         <v>966870140</v>
@@ -1547,16 +1541,16 @@
         <v>3009233</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>248</v>
+        <v>242</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>249</v>
+        <v>243</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>250</v>
+        <v>244</v>
       </c>
       <c r="F12" s="3">
         <v>965823080</v>
@@ -1567,16 +1561,16 @@
         <v>3010132</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="F13" s="3">
         <v>966870700</v>
@@ -1587,16 +1581,16 @@
         <v>3010144</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>122</v>
+        <v>116</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="F14" s="3">
         <v>966912245</v>
@@ -1607,16 +1601,16 @@
         <v>3011070</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>171</v>
+        <v>165</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>172</v>
+        <v>166</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
       <c r="F15" s="3">
         <v>966904725</v>
@@ -1627,16 +1621,16 @@
         <v>3012165</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="F16" s="3">
         <v>966527660</v>
@@ -1647,16 +1641,16 @@
         <v>3012736</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="F17" s="3">
         <v>965936520</v>
@@ -1667,16 +1661,16 @@
         <v>3012785</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>154</v>
+        <v>148</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>155</v>
+        <v>149</v>
       </c>
       <c r="F18" s="3">
         <v>966957290</v>
@@ -1687,16 +1681,16 @@
         <v>3013224</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="F19" s="3">
         <v>966912260</v>
@@ -1707,16 +1701,16 @@
         <v>3013339</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>251</v>
+        <v>245</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>252</v>
+        <v>246</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>253</v>
+        <v>247</v>
       </c>
       <c r="F20" s="3">
         <v>966428205</v>
@@ -1727,16 +1721,16 @@
         <v>3013716</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="F21" s="3">
         <v>966870935</v>
@@ -1747,16 +1741,16 @@
         <v>3013728</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>185</v>
+        <v>179</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>186</v>
+        <v>180</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>187</v>
+        <v>181</v>
       </c>
       <c r="F22" s="3">
         <v>966904735</v>
@@ -1767,16 +1761,16 @@
         <v>3013819</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="F23" s="3">
         <v>965936540</v>
@@ -1787,16 +1781,16 @@
         <v>3014371</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>182</v>
+        <v>176</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>183</v>
+        <v>177</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>184</v>
+        <v>178</v>
       </c>
       <c r="F24" s="3">
         <v>966957300</v>
@@ -1807,16 +1801,16 @@
         <v>3014551</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>159</v>
+        <v>153</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c r="E25" s="3" t="s">
-        <v>161</v>
+        <v>155</v>
       </c>
       <c r="F25" s="3">
         <v>965936475</v>
@@ -1827,16 +1821,16 @@
         <v>3014800</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="E26" s="3" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="F26" s="3">
         <v>966912295</v>
@@ -1847,16 +1841,16 @@
         <v>3014812</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="E27" s="3" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
       <c r="F27" s="3">
         <v>966957330</v>
@@ -1867,36 +1861,36 @@
         <v>3014851</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>191</v>
+        <v>185</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>192</v>
+        <v>186</v>
       </c>
       <c r="E28" s="3" t="s">
-        <v>193</v>
+        <v>187</v>
       </c>
       <c r="F28" s="3">
         <v>965290210</v>
       </c>
     </row>
-    <row r="29" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="2">
         <v>3014897</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="E29" s="3" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
       <c r="F29" s="3">
         <v>965290215</v>
@@ -1907,16 +1901,16 @@
         <v>3015038</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="E30" s="3" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="F30" s="3">
         <v>965936590</v>
@@ -1927,16 +1921,16 @@
         <v>3015117</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>141</v>
+        <v>135</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>142</v>
+        <v>136</v>
       </c>
       <c r="E31" s="3" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
       <c r="F31" s="3">
         <v>966870135</v>
@@ -1947,36 +1941,36 @@
         <v>3015543</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="E32" s="3" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="F32" s="3">
         <v>965936530</v>
       </c>
     </row>
-    <row r="33" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" s="2">
         <v>3016596</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>211</v>
+        <v>205</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="D33" s="3" t="s">
-        <v>212</v>
+        <v>206</v>
       </c>
       <c r="E33" s="3" t="s">
-        <v>213</v>
+        <v>207</v>
       </c>
       <c r="F33" s="3">
         <v>966926830</v>
@@ -1987,16 +1981,16 @@
         <v>12000251</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="D34" s="3" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="E34" s="3" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="F34" s="3">
         <v>964738925</v>
@@ -2007,16 +2001,16 @@
         <v>12000406</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="D35" s="3" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="E35" s="3" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="F35" s="3">
         <v>964738930</v>
@@ -2027,16 +2021,16 @@
         <v>12000704</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="D36" s="3" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="E36" s="3" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="F36" s="3">
         <v>964738935</v>
@@ -2047,16 +2041,16 @@
         <v>12001228</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="D37" s="3" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="E37" s="3" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="F37" s="3">
         <v>964738965</v>
@@ -2067,16 +2061,16 @@
         <v>12003390</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="D38" s="3" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="E38" s="3" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="F38" s="3">
         <v>964405640</v>
@@ -2087,16 +2081,16 @@
         <v>12003444</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>245</v>
+        <v>239</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="D39" s="3" t="s">
-        <v>246</v>
+        <v>240</v>
       </c>
       <c r="E39" s="3" t="s">
-        <v>247</v>
+        <v>241</v>
       </c>
       <c r="F39" s="3">
         <v>964738985</v>
@@ -2107,16 +2101,16 @@
         <v>12004011</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="D40" s="3" t="s">
-        <v>139</v>
+        <v>133</v>
       </c>
       <c r="E40" s="3" t="s">
-        <v>140</v>
+        <v>134</v>
       </c>
       <c r="F40" s="3">
         <v>964738940</v>
@@ -2127,16 +2121,16 @@
         <v>12004217</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="C41" s="3" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="D41" s="3" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="E41" s="3" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="F41" s="3">
         <v>964738995</v>
@@ -2147,36 +2141,36 @@
         <v>12004400</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>197</v>
+        <v>191</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="D42" s="3" t="s">
-        <v>198</v>
+        <v>192</v>
       </c>
       <c r="E42" s="3" t="s">
-        <v>199</v>
+        <v>193</v>
       </c>
       <c r="F42" s="3">
         <v>964336090</v>
       </c>
     </row>
-    <row r="43" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" s="2">
         <v>12005544</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>242</v>
+        <v>236</v>
       </c>
       <c r="C43" s="3" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="D43" s="3" t="s">
-        <v>243</v>
+        <v>237</v>
       </c>
       <c r="E43" s="3" t="s">
-        <v>244</v>
+        <v>238</v>
       </c>
       <c r="F43" s="3">
         <v>964739750</v>
@@ -2187,16 +2181,16 @@
         <v>12005741</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
       <c r="C44" s="3" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="D44" s="3" t="s">
-        <v>166</v>
+        <v>160</v>
       </c>
       <c r="E44" s="3" t="s">
-        <v>167</v>
+        <v>161</v>
       </c>
       <c r="F44" s="3">
         <v>964399025</v>
@@ -2207,16 +2201,16 @@
         <v>12005751</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
       <c r="C45" s="3" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="D45" s="3" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="E45" s="3" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="F45" s="3">
         <v>964738955</v>
@@ -2227,16 +2221,16 @@
         <v>46000161</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="C46" s="3" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="D46" s="3" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="E46" s="3" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="F46" s="3">
         <v>961206150</v>
@@ -2247,16 +2241,16 @@
         <v>46000754</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="C47" s="3" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="D47" s="3" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="E47" s="3" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="F47" s="3">
         <v>962457815</v>
@@ -2267,16 +2261,16 @@
         <v>46001199</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="C48" s="3" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="D48" s="3" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="E48" s="3" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="F48" s="3">
         <v>962457820</v>
@@ -2287,16 +2281,16 @@
         <v>46002775</v>
       </c>
       <c r="B49" s="3" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="C49" s="3" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="D49" s="3" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="E49" s="3" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="F49" s="3">
         <v>962980130</v>
@@ -2307,16 +2301,16 @@
         <v>46003408</v>
       </c>
       <c r="B50" s="3" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="C50" s="3" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="D50" s="3" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
       <c r="E50" s="3" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="F50" s="3">
         <v>961719100</v>
@@ -2327,16 +2321,16 @@
         <v>46004221</v>
       </c>
       <c r="B51" s="3" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="C51" s="3" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="D51" s="3" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="E51" s="3" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
       <c r="F51" s="3">
         <v>962829430</v>
@@ -2347,16 +2341,16 @@
         <v>46005132</v>
       </c>
       <c r="B52" s="3" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
       <c r="C52" s="3" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="D52" s="3" t="s">
-        <v>148</v>
+        <v>142</v>
       </c>
       <c r="E52" s="3" t="s">
-        <v>149</v>
+        <v>143</v>
       </c>
       <c r="F52" s="3">
         <v>961206040</v>
@@ -2367,16 +2361,16 @@
         <v>46006100</v>
       </c>
       <c r="B53" s="3" t="s">
-        <v>168</v>
+        <v>162</v>
       </c>
       <c r="C53" s="3" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="D53" s="3" t="s">
-        <v>169</v>
+        <v>163</v>
       </c>
       <c r="E53" s="3" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="F53" s="3">
         <v>962919375</v>
@@ -2387,16 +2381,16 @@
         <v>46007748</v>
       </c>
       <c r="B54" s="3" t="s">
-        <v>194</v>
+        <v>188</v>
       </c>
       <c r="C54" s="3" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="D54" s="3" t="s">
-        <v>195</v>
+        <v>189</v>
       </c>
       <c r="E54" s="3" t="s">
-        <v>196</v>
+        <v>190</v>
       </c>
       <c r="F54" s="3">
         <v>962617720</v>
@@ -2407,16 +2401,16 @@
         <v>46007943</v>
       </c>
       <c r="B55" s="3" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="C55" s="3" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="D55" s="3" t="s">
-        <v>203</v>
+        <v>197</v>
       </c>
       <c r="E55" s="3" t="s">
-        <v>204</v>
+        <v>198</v>
       </c>
       <c r="F55" s="3">
         <v>961206160</v>
@@ -2427,16 +2421,16 @@
         <v>46008340</v>
       </c>
       <c r="B56" s="3" t="s">
-        <v>205</v>
+        <v>199</v>
       </c>
       <c r="C56" s="3" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="D56" s="3" t="s">
-        <v>206</v>
+        <v>200</v>
       </c>
       <c r="E56" s="3" t="s">
-        <v>207</v>
+        <v>201</v>
       </c>
       <c r="F56" s="3">
         <v>962829995</v>
@@ -2447,16 +2441,16 @@
         <v>46008972</v>
       </c>
       <c r="B57" s="3" t="s">
-        <v>214</v>
+        <v>208</v>
       </c>
       <c r="C57" s="3" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="D57" s="3" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
       <c r="E57" s="3" t="s">
-        <v>216</v>
+        <v>210</v>
       </c>
       <c r="F57" s="3">
         <v>962169255</v>
@@ -2467,16 +2461,16 @@
         <v>46012963</v>
       </c>
       <c r="B58" s="3" t="s">
-        <v>236</v>
+        <v>230</v>
       </c>
       <c r="C58" s="3" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="D58" s="3" t="s">
-        <v>237</v>
+        <v>231</v>
       </c>
       <c r="E58" s="3" t="s">
-        <v>238</v>
+        <v>232</v>
       </c>
       <c r="F58" s="3">
         <v>961206045</v>
@@ -2487,16 +2481,16 @@
         <v>46013086</v>
       </c>
       <c r="B59" s="3" t="s">
-        <v>231</v>
+        <v>225</v>
       </c>
       <c r="C59" s="3" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="D59" s="3" t="s">
-        <v>232</v>
+        <v>226</v>
       </c>
       <c r="E59" s="3" t="s">
-        <v>228</v>
+        <v>222</v>
       </c>
       <c r="F59" s="3">
         <v>961206190</v>
@@ -2507,16 +2501,16 @@
         <v>46014224</v>
       </c>
       <c r="B60" s="3" t="s">
-        <v>229</v>
+        <v>223</v>
       </c>
       <c r="C60" s="3" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="D60" s="3" t="s">
-        <v>230</v>
+        <v>224</v>
       </c>
       <c r="E60" s="3" t="s">
-        <v>219</v>
+        <v>213</v>
       </c>
       <c r="F60" s="3">
         <v>961206065</v>
@@ -2527,16 +2521,16 @@
         <v>46015290</v>
       </c>
       <c r="B61" s="3" t="s">
-        <v>226</v>
+        <v>220</v>
       </c>
       <c r="C61" s="3" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="D61" s="3" t="s">
-        <v>227</v>
+        <v>221</v>
       </c>
       <c r="E61" s="3" t="s">
-        <v>228</v>
+        <v>222</v>
       </c>
       <c r="F61" s="3">
         <v>961206030</v>
@@ -2547,16 +2541,16 @@
         <v>46015733</v>
       </c>
       <c r="B62" s="3" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="C62" s="3" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="D62" s="3" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="E62" s="3" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="F62" s="3">
         <v>961892940</v>
@@ -2567,16 +2561,16 @@
         <v>46016038</v>
       </c>
       <c r="B63" s="3" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="C63" s="3" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="D63" s="3" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="E63" s="3" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="F63" s="3">
         <v>961206210</v>
@@ -2587,36 +2581,36 @@
         <v>46016312</v>
       </c>
       <c r="B64" s="3" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="C64" s="3" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="D64" s="3" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="E64" s="3" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="F64" s="3">
         <v>961719085</v>
       </c>
     </row>
-    <row r="65" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A65" s="2">
         <v>46016440</v>
       </c>
       <c r="B65" s="3" t="s">
-        <v>257</v>
+        <v>251</v>
       </c>
       <c r="C65" s="3" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="D65" s="3" t="s">
-        <v>258</v>
+        <v>252</v>
       </c>
       <c r="E65" s="3" t="s">
-        <v>259</v>
+        <v>253</v>
       </c>
       <c r="F65" s="3">
         <v>961206075</v>
@@ -2627,16 +2621,16 @@
         <v>46017675</v>
       </c>
       <c r="B66" s="3" t="s">
-        <v>174</v>
+        <v>168</v>
       </c>
       <c r="C66" s="3" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="D66" s="3" t="s">
-        <v>175</v>
+        <v>169</v>
       </c>
       <c r="E66" s="3" t="s">
-        <v>176</v>
+        <v>170</v>
       </c>
       <c r="F66" s="3">
         <v>961205955</v>
@@ -2647,76 +2641,76 @@
         <v>46017882</v>
       </c>
       <c r="B67" s="3" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="C67" s="3" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="D67" s="3" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="E67" s="3" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="F67" s="3">
         <v>961606970</v>
       </c>
     </row>
-    <row r="68" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A68" s="2">
         <v>46018692</v>
       </c>
       <c r="B68" s="3" t="s">
-        <v>254</v>
+        <v>248</v>
       </c>
       <c r="C68" s="3" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="D68" s="3" t="s">
-        <v>255</v>
+        <v>249</v>
       </c>
       <c r="E68" s="3" t="s">
-        <v>256</v>
+        <v>250</v>
       </c>
       <c r="F68" s="3">
         <v>962249080</v>
       </c>
     </row>
-    <row r="69" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A69" s="2">
         <v>46018692</v>
       </c>
       <c r="B69" s="3" t="s">
-        <v>254</v>
+        <v>248</v>
       </c>
       <c r="C69" s="3" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="D69" s="3" t="s">
-        <v>263</v>
+        <v>257</v>
       </c>
       <c r="E69" s="3" t="s">
-        <v>256</v>
+        <v>250</v>
       </c>
       <c r="F69" s="3">
         <v>962249080</v>
       </c>
     </row>
-    <row r="70" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A70" s="2">
         <v>46018761</v>
       </c>
       <c r="B70" s="3" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="C70" s="3" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="D70" s="3" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="E70" s="3" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="F70" s="3">
         <v>962787530</v>
@@ -2727,16 +2721,16 @@
         <v>46019015</v>
       </c>
       <c r="B71" s="3" t="s">
-        <v>208</v>
+        <v>202</v>
       </c>
       <c r="C71" s="3" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="D71" s="3" t="s">
-        <v>209</v>
+        <v>203</v>
       </c>
       <c r="E71" s="3" t="s">
-        <v>210</v>
+        <v>204</v>
       </c>
       <c r="F71" s="3">
         <v>961206090</v>
@@ -2747,16 +2741,16 @@
         <v>46019660</v>
       </c>
       <c r="B72" s="3" t="s">
-        <v>150</v>
+        <v>144</v>
       </c>
       <c r="C72" s="3" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="D72" s="3" t="s">
-        <v>151</v>
+        <v>145</v>
       </c>
       <c r="E72" s="3" t="s">
-        <v>152</v>
+        <v>146</v>
       </c>
       <c r="F72" s="3">
         <v>961205925</v>
@@ -2767,16 +2761,16 @@
         <v>46019763</v>
       </c>
       <c r="B73" s="3" t="s">
-        <v>233</v>
+        <v>227</v>
       </c>
       <c r="C73" s="3" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="D73" s="3" t="s">
-        <v>234</v>
+        <v>228</v>
       </c>
       <c r="E73" s="3" t="s">
-        <v>235</v>
+        <v>229</v>
       </c>
       <c r="F73" s="3">
         <v>961206255</v>
@@ -2787,16 +2781,16 @@
         <v>46020315</v>
       </c>
       <c r="B74" s="3" t="s">
-        <v>188</v>
+        <v>182</v>
       </c>
       <c r="C74" s="3" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="D74" s="3" t="s">
-        <v>189</v>
+        <v>183</v>
       </c>
       <c r="E74" s="3" t="s">
-        <v>190</v>
+        <v>184</v>
       </c>
       <c r="F74" s="3">
         <v>961205985</v>
@@ -2807,16 +2801,16 @@
         <v>46020479</v>
       </c>
       <c r="B75" s="3" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="C75" s="3" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="D75" s="3" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="E75" s="3" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="F75" s="3">
         <v>962829400</v>
@@ -2827,16 +2821,16 @@
         <v>46020480</v>
       </c>
       <c r="B76" s="3" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="C76" s="3" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="D76" s="3" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="E76" s="3" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="F76" s="3">
         <v>962249055</v>
@@ -2847,16 +2841,16 @@
         <v>46021290</v>
       </c>
       <c r="B77" s="3" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="C77" s="3" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="D77" s="3" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="E77" s="3" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="F77" s="3">
         <v>962457865</v>
@@ -2867,16 +2861,16 @@
         <v>46021711</v>
       </c>
       <c r="B78" s="3" t="s">
-        <v>217</v>
+        <v>211</v>
       </c>
       <c r="C78" s="3" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="D78" s="3" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="E78" s="3" t="s">
-        <v>219</v>
+        <v>213</v>
       </c>
       <c r="F78" s="3">
         <v>961205930</v>
@@ -2887,16 +2881,16 @@
         <v>46022099</v>
       </c>
       <c r="B79" s="3" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="C79" s="3" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="D79" s="3" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="E79" s="3" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="F79" s="3">
         <v>962919595</v>
@@ -2907,16 +2901,16 @@
         <v>46022129</v>
       </c>
       <c r="B80" s="3" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="C80" s="3" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="D80" s="3" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="E80" s="3" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="F80" s="3">
         <v>962829415</v>
@@ -2927,16 +2921,16 @@
         <v>46022257</v>
       </c>
       <c r="B81" s="3" t="s">
-        <v>223</v>
+        <v>217</v>
       </c>
       <c r="C81" s="3" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="D81" s="3" t="s">
-        <v>224</v>
+        <v>218</v>
       </c>
       <c r="E81" s="3" t="s">
-        <v>225</v>
+        <v>219</v>
       </c>
       <c r="F81" s="3">
         <v>961206100</v>
@@ -2947,16 +2941,16 @@
         <v>46022543</v>
       </c>
       <c r="B82" s="3" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
       <c r="C82" s="3" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="D82" s="3" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
       <c r="E82" s="3" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
       <c r="F82" s="3">
         <v>962718345</v>
@@ -2967,16 +2961,16 @@
         <v>46022622</v>
       </c>
       <c r="B83" s="3" t="s">
-        <v>177</v>
+        <v>171</v>
       </c>
       <c r="C83" s="3" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="D83" s="3" t="s">
-        <v>178</v>
+        <v>172</v>
       </c>
       <c r="E83" s="3" t="s">
-        <v>179</v>
+        <v>173</v>
       </c>
       <c r="F83" s="3">
         <v>961206280</v>
@@ -2987,16 +2981,16 @@
         <v>46022646</v>
       </c>
       <c r="B84" s="3" t="s">
-        <v>239</v>
+        <v>233</v>
       </c>
       <c r="C84" s="3" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="D84" s="3" t="s">
-        <v>240</v>
+        <v>234</v>
       </c>
       <c r="E84" s="3" t="s">
-        <v>241</v>
+        <v>235</v>
       </c>
       <c r="F84" s="3">
         <v>961206105</v>
@@ -3007,16 +3001,16 @@
         <v>46023250</v>
       </c>
       <c r="B85" s="3" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="C85" s="3" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="D85" s="3" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="E85" s="3" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="F85" s="3">
         <v>962980140</v>
@@ -3027,16 +3021,16 @@
         <v>46023924</v>
       </c>
       <c r="B86" s="3" t="s">
-        <v>156</v>
+        <v>150</v>
       </c>
       <c r="C86" s="3" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="D86" s="3" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
       <c r="E86" s="3" t="s">
-        <v>158</v>
+        <v>152</v>
       </c>
       <c r="F86" s="3">
         <v>962980145</v>
@@ -3047,16 +3041,16 @@
         <v>46024424</v>
       </c>
       <c r="B87" s="3" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="C87" s="3" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="D87" s="3" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="E87" s="3" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="F87" s="3">
         <v>961207330</v>
@@ -3067,36 +3061,36 @@
         <v>46025040</v>
       </c>
       <c r="B88" s="3" t="s">
-        <v>220</v>
+        <v>214</v>
       </c>
       <c r="C88" s="3" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="D88" s="3" t="s">
-        <v>221</v>
+        <v>215</v>
       </c>
       <c r="E88" s="3" t="s">
-        <v>222</v>
+        <v>216</v>
       </c>
       <c r="F88" s="3">
         <v>961205875</v>
       </c>
     </row>
-    <row r="89" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A89" s="2">
         <v>46025799</v>
       </c>
       <c r="B89" s="3" t="s">
-        <v>260</v>
+        <v>254</v>
       </c>
       <c r="C89" s="3" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="D89" s="3" t="s">
-        <v>261</v>
+        <v>255</v>
       </c>
       <c r="E89" s="3" t="s">
-        <v>262</v>
+        <v>256</v>
       </c>
       <c r="F89" s="3">
         <v>961206990</v>

</xml_diff>